<commit_message>
New build, fixed Format tag
</commit_message>
<xml_diff>
--- a/pyduq/tests/counters.xlsx
+++ b/pyduq/tests/counters.xlsx
@@ -46491,7 +46491,7 @@
     <row r="2095">
       <c r="A2095" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2095" t="inlineStr">
@@ -46501,19 +46501,19 @@
       </c>
       <c r="C2095" t="inlineStr">
         <is>
-          <t>Error: Value '5/02/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'SMITHFIELD PLAINS  SA  5114' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2095" t="inlineStr">
         <is>
-          <t>Row: 173</t>
+          <t>Row: 34</t>
         </is>
       </c>
     </row>
     <row r="2096">
       <c r="A2096" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2096" t="inlineStr">
@@ -46523,19 +46523,19 @@
       </c>
       <c r="C2096" t="inlineStr">
         <is>
-          <t>Error: Value '3/05/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'SMITHFIELD PLAINS  SA  5114' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2096" t="inlineStr">
         <is>
-          <t>Row: 692</t>
+          <t>Row: 43</t>
         </is>
       </c>
     </row>
     <row r="2097">
       <c r="A2097" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2097" t="inlineStr">
@@ -46545,19 +46545,19 @@
       </c>
       <c r="C2097" t="inlineStr">
         <is>
-          <t>Error: Value '9/06/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2097" t="inlineStr">
         <is>
-          <t>Row: 974</t>
+          <t>Row: 89</t>
         </is>
       </c>
     </row>
     <row r="2098">
       <c r="A2098" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2098" t="inlineStr">
@@ -46567,19 +46567,19 @@
       </c>
       <c r="C2098" t="inlineStr">
         <is>
-          <t>Error: Value '3/09/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2098" t="inlineStr">
         <is>
-          <t>Row: 1704</t>
+          <t>Row: 190</t>
         </is>
       </c>
     </row>
     <row r="2099">
       <c r="A2099" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2099" t="inlineStr">
@@ -46589,19 +46589,19 @@
       </c>
       <c r="C2099" t="inlineStr">
         <is>
-          <t>Error: Value '4/09/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'GULFVIEW HEIGHTS  SA  5096' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2099" t="inlineStr">
         <is>
-          <t>Row: 1712</t>
+          <t>Row: 217</t>
         </is>
       </c>
     </row>
     <row r="2100">
       <c r="A2100" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2100" t="inlineStr">
@@ -46611,19 +46611,19 @@
       </c>
       <c r="C2100" t="inlineStr">
         <is>
-          <t>Error: Value '6/11/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2100" t="inlineStr">
         <is>
-          <t>Row: 2370</t>
+          <t>Row: 227</t>
         </is>
       </c>
     </row>
     <row r="2101">
       <c r="A2101" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2101" t="inlineStr">
@@ -46633,19 +46633,19 @@
       </c>
       <c r="C2101" t="inlineStr">
         <is>
-          <t>Error: Value '6/11/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2101" t="inlineStr">
         <is>
-          <t>Row: 2371</t>
+          <t>Row: 228</t>
         </is>
       </c>
     </row>
     <row r="2102">
       <c r="A2102" t="inlineStr">
         <is>
-          <t>CertifierLodgementDates</t>
+          <t>ApplicantAddressLine3</t>
         </is>
       </c>
       <c r="B2102" t="inlineStr">
@@ -46655,32 +46655,2826 @@
       </c>
       <c r="C2102" t="inlineStr">
         <is>
-          <t>Error: Value '3/12/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
         </is>
       </c>
       <c r="D2102" t="inlineStr">
         <is>
-          <t>Row: 2659</t>
+          <t>Row: 463</t>
         </is>
       </c>
     </row>
     <row r="2103">
       <c r="A2103" t="inlineStr">
         <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2103" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2103" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2103" t="inlineStr">
+        <is>
+          <t>Row: 470</t>
+        </is>
+      </c>
+    </row>
+    <row r="2104">
+      <c r="A2104" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2104" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2104" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2104" t="inlineStr">
+        <is>
+          <t>Row: 483</t>
+        </is>
+      </c>
+    </row>
+    <row r="2105">
+      <c r="A2105" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2105" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2105" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2105" t="inlineStr">
+        <is>
+          <t>Row: 531</t>
+        </is>
+      </c>
+    </row>
+    <row r="2106">
+      <c r="A2106" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2106" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2106" t="inlineStr">
+        <is>
+          <t>Error: Value 'BALGOWLAH HEIGHTS  NSW  2093' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2106" t="inlineStr">
+        <is>
+          <t>Row: 596</t>
+        </is>
+      </c>
+    </row>
+    <row r="2107">
+      <c r="A2107" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2107" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2107" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2107" t="inlineStr">
+        <is>
+          <t>Row: 671</t>
+        </is>
+      </c>
+    </row>
+    <row r="2108">
+      <c r="A2108" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2108" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2108" t="inlineStr">
+        <is>
+          <t>Error: Value 'MUNNO PARA DOWNS  SA  5115' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2108" t="inlineStr">
+        <is>
+          <t>Row: 740</t>
+        </is>
+      </c>
+    </row>
+    <row r="2109">
+      <c r="A2109" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2109" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2109" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK SOUTH  SA  5113' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2109" t="inlineStr">
+        <is>
+          <t>Row: 743</t>
+        </is>
+      </c>
+    </row>
+    <row r="2110">
+      <c r="A2110" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2110" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2110" t="inlineStr">
+        <is>
+          <t>Error: Value 'O'SULLIVAN BEACH  SA  5166' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2110" t="inlineStr">
+        <is>
+          <t>Row: 745</t>
+        </is>
+      </c>
+    </row>
+    <row r="2111">
+      <c r="A2111" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2111" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2111" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2111" t="inlineStr">
+        <is>
+          <t>Row: 759</t>
+        </is>
+      </c>
+    </row>
+    <row r="2112">
+      <c r="A2112" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2112" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2112" t="inlineStr">
+        <is>
+          <t>Error: Value '*****************************' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2112" t="inlineStr">
+        <is>
+          <t>Row: 798</t>
+        </is>
+      </c>
+    </row>
+    <row r="2113">
+      <c r="A2113" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2113" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2113" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2113" t="inlineStr">
+        <is>
+          <t>Row: 846</t>
+        </is>
+      </c>
+    </row>
+    <row r="2114">
+      <c r="A2114" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2114" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2114" t="inlineStr">
+        <is>
+          <t>Error: Value 'SALISBURY HEIGHTS  SA  5109' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2114" t="inlineStr">
+        <is>
+          <t>Row: 885</t>
+        </is>
+      </c>
+    </row>
+    <row r="2115">
+      <c r="A2115" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2115" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2115" t="inlineStr">
+        <is>
+          <t>Error: Value 'SALISBURY HEIGHTS  SA  5109' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2115" t="inlineStr">
+        <is>
+          <t>Row: 1033</t>
+        </is>
+      </c>
+    </row>
+    <row r="2116">
+      <c r="A2116" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2116" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2116" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2116" t="inlineStr">
+        <is>
+          <t>Row: 1055</t>
+        </is>
+      </c>
+    </row>
+    <row r="2117">
+      <c r="A2117" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2117" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2117" t="inlineStr">
+        <is>
+          <t>Error: Value 'HAMPSTEAD GARDENS  SA  5086' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2117" t="inlineStr">
+        <is>
+          <t>Row: 1121</t>
+        </is>
+      </c>
+    </row>
+    <row r="2118">
+      <c r="A2118" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2118" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2118" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2118" t="inlineStr">
+        <is>
+          <t>Row: 1156</t>
+        </is>
+      </c>
+    </row>
+    <row r="2119">
+      <c r="A2119" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2119" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2119" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2119" t="inlineStr">
+        <is>
+          <t>Row: 1179</t>
+        </is>
+      </c>
+    </row>
+    <row r="2120">
+      <c r="A2120" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2120" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2120" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2120" t="inlineStr">
+        <is>
+          <t>Row: 1292</t>
+        </is>
+      </c>
+    </row>
+    <row r="2121">
+      <c r="A2121" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2121" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2121" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2121" t="inlineStr">
+        <is>
+          <t>Row: 1332</t>
+        </is>
+      </c>
+    </row>
+    <row r="2122">
+      <c r="A2122" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2122" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2122" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2122" t="inlineStr">
+        <is>
+          <t>Row: 1369</t>
+        </is>
+      </c>
+    </row>
+    <row r="2123">
+      <c r="A2123" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2123" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2123" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2123" t="inlineStr">
+        <is>
+          <t>Row: 1462</t>
+        </is>
+      </c>
+    </row>
+    <row r="2124">
+      <c r="A2124" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2124" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2124" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2124" t="inlineStr">
+        <is>
+          <t>Row: 1474</t>
+        </is>
+      </c>
+    </row>
+    <row r="2125">
+      <c r="A2125" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2125" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2125" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2125" t="inlineStr">
+        <is>
+          <t>Row: 1502</t>
+        </is>
+      </c>
+    </row>
+    <row r="2126">
+      <c r="A2126" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2126" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2126" t="inlineStr">
+        <is>
+          <t>Error: Value 'MUNNO PARA DOWNS  SA  5115' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2126" t="inlineStr">
+        <is>
+          <t>Row: 1518</t>
+        </is>
+      </c>
+    </row>
+    <row r="2127">
+      <c r="A2127" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2127" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2127" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2127" t="inlineStr">
+        <is>
+          <t>Row: 1605</t>
+        </is>
+      </c>
+    </row>
+    <row r="2128">
+      <c r="A2128" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2128" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2128" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2128" t="inlineStr">
+        <is>
+          <t>Row: 1621</t>
+        </is>
+      </c>
+    </row>
+    <row r="2129">
+      <c r="A2129" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2129" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2129" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2129" t="inlineStr">
+        <is>
+          <t>Row: 1622</t>
+        </is>
+      </c>
+    </row>
+    <row r="2130">
+      <c r="A2130" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2130" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2130" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2130" t="inlineStr">
+        <is>
+          <t>Row: 1644</t>
+        </is>
+      </c>
+    </row>
+    <row r="2131">
+      <c r="A2131" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2131" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2131" t="inlineStr">
+        <is>
+          <t>Error: Value 'SALISBURY HEIGHTS  SA  5109' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2131" t="inlineStr">
+        <is>
+          <t>Row: 1651</t>
+        </is>
+      </c>
+    </row>
+    <row r="2132">
+      <c r="A2132" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2132" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2132" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2132" t="inlineStr">
+        <is>
+          <t>Row: 1666</t>
+        </is>
+      </c>
+    </row>
+    <row r="2133">
+      <c r="A2133" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2133" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2133" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2133" t="inlineStr">
+        <is>
+          <t>Row: 1686</t>
+        </is>
+      </c>
+    </row>
+    <row r="2134">
+      <c r="A2134" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2134" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2134" t="inlineStr">
+        <is>
+          <t>Error: Value 'FORTITUDE VALLEY  QLD  4006' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2134" t="inlineStr">
+        <is>
+          <t>Row: 1847</t>
+        </is>
+      </c>
+    </row>
+    <row r="2135">
+      <c r="A2135" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2135" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2135" t="inlineStr">
+        <is>
+          <t>Error: Value 'FORTITUDE VALLEY  QLD  4006' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2135" t="inlineStr">
+        <is>
+          <t>Row: 1848</t>
+        </is>
+      </c>
+    </row>
+    <row r="2136">
+      <c r="A2136" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2136" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2136" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2136" t="inlineStr">
+        <is>
+          <t>Row: 1888</t>
+        </is>
+      </c>
+    </row>
+    <row r="2137">
+      <c r="A2137" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2137" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2137" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2137" t="inlineStr">
+        <is>
+          <t>Row: 1889</t>
+        </is>
+      </c>
+    </row>
+    <row r="2138">
+      <c r="A2138" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2138" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2138" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2138" t="inlineStr">
+        <is>
+          <t>Row: 1890</t>
+        </is>
+      </c>
+    </row>
+    <row r="2139">
+      <c r="A2139" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2139" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2139" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2139" t="inlineStr">
+        <is>
+          <t>Row: 1891</t>
+        </is>
+      </c>
+    </row>
+    <row r="2140">
+      <c r="A2140" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2140" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2140" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2140" t="inlineStr">
+        <is>
+          <t>Row: 1892</t>
+        </is>
+      </c>
+    </row>
+    <row r="2141">
+      <c r="A2141" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2141" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2141" t="inlineStr">
+        <is>
+          <t>Error: Value 'SALISBURY HEIGHTS  SA  5109' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2141" t="inlineStr">
+        <is>
+          <t>Row: 1909</t>
+        </is>
+      </c>
+    </row>
+    <row r="2142">
+      <c r="A2142" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2142" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2142" t="inlineStr">
+        <is>
+          <t>Error: Value 'SMITHFIELD PLAINS  SA  5114' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2142" t="inlineStr">
+        <is>
+          <t>Row: 1964</t>
+        </is>
+      </c>
+    </row>
+    <row r="2143">
+      <c r="A2143" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2143" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2143" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2143" t="inlineStr">
+        <is>
+          <t>Row: 1986</t>
+        </is>
+      </c>
+    </row>
+    <row r="2144">
+      <c r="A2144" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2144" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2144" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2144" t="inlineStr">
+        <is>
+          <t>Row: 2038</t>
+        </is>
+      </c>
+    </row>
+    <row r="2145">
+      <c r="A2145" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2145" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2145" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLOISTERS SQUARE  WA  6850' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2145" t="inlineStr">
+        <is>
+          <t>Row: 2071</t>
+        </is>
+      </c>
+    </row>
+    <row r="2146">
+      <c r="A2146" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2146" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2146" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2146" t="inlineStr">
+        <is>
+          <t>Row: 2089</t>
+        </is>
+      </c>
+    </row>
+    <row r="2147">
+      <c r="A2147" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2147" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2147" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2147" t="inlineStr">
+        <is>
+          <t>Row: 2137</t>
+        </is>
+      </c>
+    </row>
+    <row r="2148">
+      <c r="A2148" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2148" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2148" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2148" t="inlineStr">
+        <is>
+          <t>Row: 2207</t>
+        </is>
+      </c>
+    </row>
+    <row r="2149">
+      <c r="A2149" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2149" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2149" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2149" t="inlineStr">
+        <is>
+          <t>Row: 2214</t>
+        </is>
+      </c>
+    </row>
+    <row r="2150">
+      <c r="A2150" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2150" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2150" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2150" t="inlineStr">
+        <is>
+          <t>Row: 2228</t>
+        </is>
+      </c>
+    </row>
+    <row r="2151">
+      <c r="A2151" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2151" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2151" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2151" t="inlineStr">
+        <is>
+          <t>Row: 2247</t>
+        </is>
+      </c>
+    </row>
+    <row r="2152">
+      <c r="A2152" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2152" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2152" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2152" t="inlineStr">
+        <is>
+          <t>Row: 2304</t>
+        </is>
+      </c>
+    </row>
+    <row r="2153">
+      <c r="A2153" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2153" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2153" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2153" t="inlineStr">
+        <is>
+          <t>Row: 2306</t>
+        </is>
+      </c>
+    </row>
+    <row r="2154">
+      <c r="A2154" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2154" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2154" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2154" t="inlineStr">
+        <is>
+          <t>Row: 2329</t>
+        </is>
+      </c>
+    </row>
+    <row r="2155">
+      <c r="A2155" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2155" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2155" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2155" t="inlineStr">
+        <is>
+          <t>Row: 2351</t>
+        </is>
+      </c>
+    </row>
+    <row r="2156">
+      <c r="A2156" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2156" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2156" t="inlineStr">
+        <is>
+          <t>Error: Value 'SALISBURY HEIGHTS  SA  5109' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2156" t="inlineStr">
+        <is>
+          <t>Row: 2396</t>
+        </is>
+      </c>
+    </row>
+    <row r="2157">
+      <c r="A2157" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2157" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2157" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2157" t="inlineStr">
+        <is>
+          <t>Row: 2419</t>
+        </is>
+      </c>
+    </row>
+    <row r="2158">
+      <c r="A2158" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2158" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2158" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2158" t="inlineStr">
+        <is>
+          <t>Row: 2453</t>
+        </is>
+      </c>
+    </row>
+    <row r="2159">
+      <c r="A2159" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2159" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2159" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2159" t="inlineStr">
+        <is>
+          <t>Row: 2486</t>
+        </is>
+      </c>
+    </row>
+    <row r="2160">
+      <c r="A2160" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2160" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2160" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2160" t="inlineStr">
+        <is>
+          <t>Row: 2499</t>
+        </is>
+      </c>
+    </row>
+    <row r="2161">
+      <c r="A2161" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2161" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2161" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2161" t="inlineStr">
+        <is>
+          <t>Row: 2508</t>
+        </is>
+      </c>
+    </row>
+    <row r="2162">
+      <c r="A2162" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2162" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2162" t="inlineStr">
+        <is>
+          <t>Error: Value 'Level 18 25 Grenfell Street' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2162" t="inlineStr">
+        <is>
+          <t>Row: 2631</t>
+        </is>
+      </c>
+    </row>
+    <row r="2163">
+      <c r="A2163" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2163" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2163" t="inlineStr">
+        <is>
+          <t>Error: Value 'PARAFIELD GARDENS  SA  5107' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2163" t="inlineStr">
+        <is>
+          <t>Row: 2647</t>
+        </is>
+      </c>
+    </row>
+    <row r="2164">
+      <c r="A2164" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2164" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2164" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2164" t="inlineStr">
+        <is>
+          <t>Row: 2717</t>
+        </is>
+      </c>
+    </row>
+    <row r="2165">
+      <c r="A2165" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2165" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2165" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2165" t="inlineStr">
+        <is>
+          <t>Row: 2735</t>
+        </is>
+      </c>
+    </row>
+    <row r="2166">
+      <c r="A2166" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2166" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2166" t="inlineStr">
+        <is>
+          <t>Error: Value 'Level 18 25 Grenfell Street' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2166" t="inlineStr">
+        <is>
+          <t>Row: 2769</t>
+        </is>
+      </c>
+    </row>
+    <row r="2167">
+      <c r="A2167" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2167" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2167" t="inlineStr">
+        <is>
+          <t>Error: Value 'CLARENCE GARDENS  SA  5039' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2167" t="inlineStr">
+        <is>
+          <t>Row: 2773</t>
+        </is>
+      </c>
+    </row>
+    <row r="2168">
+      <c r="A2168" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2168" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2168" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2168" t="inlineStr">
+        <is>
+          <t>Row: 2801</t>
+        </is>
+      </c>
+    </row>
+    <row r="2169">
+      <c r="A2169" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2169" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2169" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2169" t="inlineStr">
+        <is>
+          <t>Row: 2824</t>
+        </is>
+      </c>
+    </row>
+    <row r="2170">
+      <c r="A2170" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2170" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2170" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2170" t="inlineStr">
+        <is>
+          <t>Row: 2825</t>
+        </is>
+      </c>
+    </row>
+    <row r="2171">
+      <c r="A2171" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2171" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2171" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2171" t="inlineStr">
+        <is>
+          <t>Row: 2826</t>
+        </is>
+      </c>
+    </row>
+    <row r="2172">
+      <c r="A2172" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2172" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2172" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2172" t="inlineStr">
+        <is>
+          <t>Row: 2827</t>
+        </is>
+      </c>
+    </row>
+    <row r="2173">
+      <c r="A2173" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2173" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2173" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2173" t="inlineStr">
+        <is>
+          <t>Row: 2828</t>
+        </is>
+      </c>
+    </row>
+    <row r="2174">
+      <c r="A2174" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2174" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2174" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2174" t="inlineStr">
+        <is>
+          <t>Row: 2829</t>
+        </is>
+      </c>
+    </row>
+    <row r="2175">
+      <c r="A2175" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2175" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2175" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2175" t="inlineStr">
+        <is>
+          <t>Row: 2830</t>
+        </is>
+      </c>
+    </row>
+    <row r="2176">
+      <c r="A2176" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2176" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2176" t="inlineStr">
+        <is>
+          <t>Error: Value 'TORRENSVILLE PLAZA  SA  5031' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2176" t="inlineStr">
+        <is>
+          <t>Row: 2831</t>
+        </is>
+      </c>
+    </row>
+    <row r="2177">
+      <c r="A2177" t="inlineStr">
+        <is>
+          <t>ApplicantAddressLine3</t>
+        </is>
+      </c>
+      <c r="B2177" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2177" t="inlineStr">
+        <is>
+          <t>Error: Value 'Suite 12,154 Fullarton Road' is longer than size '25'</t>
+        </is>
+      </c>
+      <c r="D2177" t="inlineStr">
+        <is>
+          <t>Row: 2867</t>
+        </is>
+      </c>
+    </row>
+    <row r="2178">
+      <c r="A2178" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2178" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2178" t="inlineStr">
+        <is>
+          <t>Error: Value 'crap' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2178" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2179">
+      <c r="A2179" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2179" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2179" t="inlineStr">
+        <is>
+          <t>Error: Value 'noaddress' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2179" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2180">
+      <c r="A2180" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2180" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2180" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2180" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2181">
+      <c r="A2181" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2181" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2181" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2181" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2182">
+      <c r="A2182" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2182" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2182" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2182" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2183">
+      <c r="A2183" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2183" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2183" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2183" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2184">
+      <c r="A2184" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2184" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2184" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2184" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2185">
+      <c r="A2185" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2185" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2185" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2185" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2186">
+      <c r="A2186" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2186" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2186" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2186" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2187">
+      <c r="A2187" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2187" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2187" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2187" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2188">
+      <c r="A2188" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2188" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2188" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2188" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2189">
+      <c r="A2189" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2189" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2189" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2189" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2190">
+      <c r="A2190" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2190" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2190" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2190" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2191">
+      <c r="A2191" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2191" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2191" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2191" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2192">
+      <c r="A2192" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2192" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2192" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2192" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2193">
+      <c r="A2193" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2193" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2193" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2193" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2194">
+      <c r="A2194" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2194" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2194" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2194" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2195">
+      <c r="A2195" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2195" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2195" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2195" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2196">
+      <c r="A2196" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2196" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2196" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2196" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2197">
+      <c r="A2197" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2197" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2197" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2197" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2198">
+      <c r="A2198" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2198" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2198" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2198" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2199">
+      <c r="A2199" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2199" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2199" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2199" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2200">
+      <c r="A2200" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2200" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2200" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2200" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2201">
+      <c r="A2201" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2201" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2201" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2201" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2202">
+      <c r="A2202" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2202" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2202" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2202" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2203">
+      <c r="A2203" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2203" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2203" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2203" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2204">
+      <c r="A2204" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2204" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2204" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2204" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2205">
+      <c r="A2205" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2205" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2205" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2205" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2206">
+      <c r="A2206" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2206" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2206" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2206" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2207">
+      <c r="A2207" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2207" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2207" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2207" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2208">
+      <c r="A2208" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2208" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2208" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2208" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2209">
+      <c r="A2209" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2209" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2209" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2209" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2210">
+      <c r="A2210" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2210" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2210" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2210" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2211">
+      <c r="A2211" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2211" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2211" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2211" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2212">
+      <c r="A2212" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2212" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2212" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2212" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2213">
+      <c r="A2213" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2213" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2213" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2213" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2214">
+      <c r="A2214" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2214" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2214" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2214" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2215">
+      <c r="A2215" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2215" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2215" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2215" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2216">
+      <c r="A2216" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2216" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2216" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2216" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2217">
+      <c r="A2217" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2217" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2217" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2217" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2218">
+      <c r="A2218" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2218" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2218" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2218" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2219">
+      <c r="A2219" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2219" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2219" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2219" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2220">
+      <c r="A2220" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2220" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2220" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2220" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2221">
+      <c r="A2221" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2221" t="inlineStr">
+        <is>
+          <t>Format Consistency</t>
+        </is>
+      </c>
+      <c r="C2221" t="inlineStr">
+        <is>
+          <t>Error: Value 'DAVOREN PARK  SA  5113' does not match regex #'[A-Za-z0-9._%+-]+@[A-Za-z0-9.-]+\.[A-Z|a-z]{2,7}'</t>
+        </is>
+      </c>
+      <c r="D2221" t="inlineStr">
+        <is>
+          <t>&lt;Unspecified&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2222">
+      <c r="A2222" t="inlineStr">
+        <is>
           <t>CertifierLodgementDates</t>
         </is>
       </c>
-      <c r="B2103" t="inlineStr">
+      <c r="B2222" t="inlineStr">
         <is>
           <t>Metadata Compliance</t>
         </is>
       </c>
-      <c r="C2103" t="inlineStr">
+      <c r="C2222" t="inlineStr">
+        <is>
+          <t>Error: Value '5/02/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2222" t="inlineStr">
+        <is>
+          <t>Row: 173</t>
+        </is>
+      </c>
+    </row>
+    <row r="2223">
+      <c r="A2223" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2223" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2223" t="inlineStr">
+        <is>
+          <t>Error: Value '3/05/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2223" t="inlineStr">
+        <is>
+          <t>Row: 692</t>
+        </is>
+      </c>
+    </row>
+    <row r="2224">
+      <c r="A2224" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2224" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2224" t="inlineStr">
+        <is>
+          <t>Error: Value '9/06/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2224" t="inlineStr">
+        <is>
+          <t>Row: 974</t>
+        </is>
+      </c>
+    </row>
+    <row r="2225">
+      <c r="A2225" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2225" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2225" t="inlineStr">
+        <is>
+          <t>Error: Value '3/09/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2225" t="inlineStr">
+        <is>
+          <t>Row: 1704</t>
+        </is>
+      </c>
+    </row>
+    <row r="2226">
+      <c r="A2226" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2226" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2226" t="inlineStr">
+        <is>
+          <t>Error: Value '4/09/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2226" t="inlineStr">
+        <is>
+          <t>Row: 1712</t>
+        </is>
+      </c>
+    </row>
+    <row r="2227">
+      <c r="A2227" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2227" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2227" t="inlineStr">
+        <is>
+          <t>Error: Value '6/11/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2227" t="inlineStr">
+        <is>
+          <t>Row: 2370</t>
+        </is>
+      </c>
+    </row>
+    <row r="2228">
+      <c r="A2228" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2228" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2228" t="inlineStr">
+        <is>
+          <t>Error: Value '6/11/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2228" t="inlineStr">
+        <is>
+          <t>Row: 2371</t>
+        </is>
+      </c>
+    </row>
+    <row r="2229">
+      <c r="A2229" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2229" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2229" t="inlineStr">
+        <is>
+          <t>Error: Value '3/12/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
+        </is>
+      </c>
+      <c r="D2229" t="inlineStr">
+        <is>
+          <t>Row: 2659</t>
+        </is>
+      </c>
+    </row>
+    <row r="2230">
+      <c r="A2230" t="inlineStr">
+        <is>
+          <t>CertifierLodgementDates</t>
+        </is>
+      </c>
+      <c r="B2230" t="inlineStr">
+        <is>
+          <t>Metadata Compliance</t>
+        </is>
+      </c>
+      <c r="C2230" t="inlineStr">
         <is>
           <t>Error: Value '8/12/2020' is outside the enumeration set '[',', '03/05/2020', '03/09/2020', '03/12/2020', '04/09/2020', '05/02/2020', '06/11/2020', '08/12/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '15/09/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']'</t>
         </is>
       </c>
-      <c r="D2103" t="inlineStr">
+      <c r="D2230" t="inlineStr">
         <is>
           <t>Row: 2734</t>
         </is>

</xml_diff>